<commit_message>
denoising/tied ae + beginning aae
</commit_message>
<xml_diff>
--- a/results_anomaly.xlsx
+++ b/results_anomaly.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27211"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmyara/development/me/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmyara/development/playground/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="840" windowWidth="29940" windowHeight="18320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="23">
   <si>
     <t>1. Preliminary baseline results</t>
   </si>
@@ -89,6 +86,24 @@
   </si>
   <si>
     <t>MNIST\{4}</t>
+  </si>
+  <si>
+    <t>Denoising-AE</t>
+  </si>
+  <si>
+    <t>noise=20%</t>
+  </si>
+  <si>
+    <t>possible discussion of BN vs no BN</t>
+  </si>
+  <si>
+    <t>Tied-AE (1/2 params)</t>
+  </si>
+  <si>
+    <t>Tied-AE (~#params AE)</t>
+  </si>
+  <si>
+    <t>Denoising-Tied-AE</t>
   </si>
 </sst>
 </file>
@@ -444,15 +459,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="156" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="156" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
@@ -658,7 +673,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -672,7 +687,7 @@
         <v>0.60799999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -686,7 +701,7 @@
         <v>0.52900000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -700,7 +715,7 @@
         <v>0.32900000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -711,7 +726,69 @@
         <v>14</v>
       </c>
       <c r="D20" s="3">
-        <v>0.67700000000000005</v>
+        <v>0.67800000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="E21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.61099999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23">
+        <v>0.65900000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.64700000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>